<commit_message>
C29 - Update Docker.xlsx
</commit_message>
<xml_diff>
--- a/Docker.xlsx
+++ b/Docker.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18468" windowHeight="9215" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chung" sheetId="1" r:id="rId1"/>
     <sheet name="Cài đặt (Windows)" sheetId="2" r:id="rId2"/>
+    <sheet name="Docker-Compose" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Chung!$A$1:$AC$52</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Cài đặt (Windows)'!$A$1:$AC$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Docker-Compose'!$A$1:$AC$73</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Docker</t>
   </si>
@@ -85,6 +87,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Túm lại </t>
     </r>
     <r>
@@ -140,6 +148,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>WSL</t>
     </r>
     <r>
@@ -206,6 +220,27 @@
   <si>
     <t>https://www.docker.com/</t>
   </si>
+  <si>
+    <t>Docker-Compose</t>
+  </si>
+  <si>
+    <t>What is docker-compose</t>
+  </si>
+  <si>
+    <t>Docker Compose is a tool for defining and running multi-container Docker applications</t>
+  </si>
+  <si>
+    <t>It allows developers to define a set of related services, such as web servers, databases, and other components</t>
+  </si>
+  <si>
+    <t>as single application, and then deploy and manage that application using simple command</t>
+  </si>
+  <si>
+    <t>Docker Compose uses a YAML file (*.yml) to define services, configurations and dependencies of an application</t>
+  </si>
+  <si>
+    <t>Docker Compose Component</t>
+  </si>
 </sst>
 </file>
 
@@ -217,7 +252,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,15 +290,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -273,6 +307,13 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -287,8 +328,17 @@
       <charset val="128"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,11 +351,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -319,6 +406,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,6 +441,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -355,69 +457,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -461,7 +502,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,19 +604,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,37 +652,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,97 +664,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,7 +676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,6 +725,57 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -721,53 +813,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -783,6 +850,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,73 +906,14 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -893,131 +934,131 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1058,35 +1099,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1095,22 +1139,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1343,6 +1375,53 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="497840" y="2007870"/>
+          <a:ext cx="6713220" cy="5288280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1635,7 +1714,7 @@
   <sheetPr/>
   <dimension ref="B1:AB51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" topLeftCell="A34" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1678,7 +1757,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
-      <c r="AB1" s="22"/>
+      <c r="AB1" s="15"/>
     </row>
     <row r="2" spans="2:28">
       <c r="B2" s="6"/>
@@ -1707,7 +1786,7 @@
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
-      <c r="AB2" s="23"/>
+      <c r="AB2" s="16"/>
     </row>
     <row r="3" spans="2:28">
       <c r="B3" s="6"/>
@@ -1736,11 +1815,11 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AB3" s="23"/>
+      <c r="AB3" s="16"/>
     </row>
     <row r="4" ht="20.1" customHeight="1" spans="2:28">
       <c r="B4" s="8"/>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1769,7 +1848,7 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
-      <c r="AB4" s="24"/>
+      <c r="AB4" s="17"/>
     </row>
     <row r="5" spans="2:28">
       <c r="B5" s="10"/>
@@ -1798,7 +1877,7 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
-      <c r="AB5" s="25"/>
+      <c r="AB5" s="18"/>
     </row>
     <row r="6" ht="15" spans="2:28">
       <c r="B6" s="10"/>
@@ -1831,7 +1910,7 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="12"/>
-      <c r="AB6" s="25"/>
+      <c r="AB6" s="18"/>
     </row>
     <row r="7" ht="15" spans="2:28">
       <c r="B7" s="10"/>
@@ -1864,7 +1943,7 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
-      <c r="AB7" s="25"/>
+      <c r="AB7" s="18"/>
     </row>
     <row r="8" ht="15" spans="2:28">
       <c r="B8" s="10"/>
@@ -1872,7 +1951,7 @@
       <c r="D8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="28" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="12"/>
@@ -1897,7 +1976,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
-      <c r="AB8" s="25"/>
+      <c r="AB8" s="18"/>
     </row>
     <row r="9" ht="15" spans="2:28">
       <c r="B9" s="10"/>
@@ -1905,7 +1984,7 @@
       <c r="D9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="12"/>
@@ -1930,7 +2009,7 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
       <c r="AA9" s="12"/>
-      <c r="AB9" s="25"/>
+      <c r="AB9" s="18"/>
     </row>
     <row r="10" spans="2:28">
       <c r="B10" s="10"/>
@@ -1959,11 +2038,11 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="12"/>
-      <c r="AB10" s="25"/>
+      <c r="AB10" s="18"/>
     </row>
     <row r="11" ht="20.1" customHeight="1" spans="2:28">
       <c r="B11" s="8"/>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -1992,7 +2071,7 @@
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
-      <c r="AB11" s="24"/>
+      <c r="AB11" s="17"/>
     </row>
     <row r="12" spans="2:28">
       <c r="B12" s="10"/>
@@ -2021,7 +2100,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
-      <c r="AB12" s="25"/>
+      <c r="AB12" s="18"/>
     </row>
     <row r="13" spans="2:28">
       <c r="B13" s="10"/>
@@ -2050,7 +2129,7 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
-      <c r="AB13" s="25"/>
+      <c r="AB13" s="18"/>
     </row>
     <row r="14" spans="2:28">
       <c r="B14" s="10"/>
@@ -2079,7 +2158,7 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
       <c r="AA14" s="12"/>
-      <c r="AB14" s="25"/>
+      <c r="AB14" s="18"/>
     </row>
     <row r="15" spans="2:28">
       <c r="B15" s="10"/>
@@ -2108,7 +2187,7 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
-      <c r="AB15" s="25"/>
+      <c r="AB15" s="18"/>
     </row>
     <row r="16" spans="2:28">
       <c r="B16" s="10"/>
@@ -2137,7 +2216,7 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
-      <c r="AB16" s="25"/>
+      <c r="AB16" s="18"/>
     </row>
     <row r="17" spans="2:28">
       <c r="B17" s="10"/>
@@ -2166,7 +2245,7 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
-      <c r="AB17" s="25"/>
+      <c r="AB17" s="18"/>
     </row>
     <row r="18" spans="2:28">
       <c r="B18" s="10"/>
@@ -2195,7 +2274,7 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
-      <c r="AB18" s="25"/>
+      <c r="AB18" s="18"/>
     </row>
     <row r="19" spans="2:28">
       <c r="B19" s="10"/>
@@ -2224,7 +2303,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
-      <c r="AB19" s="25"/>
+      <c r="AB19" s="18"/>
     </row>
     <row r="20" spans="2:28">
       <c r="B20" s="10"/>
@@ -2253,7 +2332,7 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
-      <c r="AB20" s="25"/>
+      <c r="AB20" s="18"/>
     </row>
     <row r="21" spans="2:28">
       <c r="B21" s="10"/>
@@ -2282,7 +2361,7 @@
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
-      <c r="AB21" s="25"/>
+      <c r="AB21" s="18"/>
     </row>
     <row r="22" spans="2:28">
       <c r="B22" s="10"/>
@@ -2311,7 +2390,7 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
-      <c r="AB22" s="25"/>
+      <c r="AB22" s="18"/>
     </row>
     <row r="23" spans="2:28">
       <c r="B23" s="10"/>
@@ -2340,7 +2419,7 @@
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
       <c r="AA23" s="12"/>
-      <c r="AB23" s="25"/>
+      <c r="AB23" s="18"/>
     </row>
     <row r="24" spans="2:28">
       <c r="B24" s="10"/>
@@ -2369,7 +2448,7 @@
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
       <c r="AA24" s="12"/>
-      <c r="AB24" s="25"/>
+      <c r="AB24" s="18"/>
     </row>
     <row r="25" spans="2:28">
       <c r="B25" s="10"/>
@@ -2398,7 +2477,7 @@
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
       <c r="AA25" s="12"/>
-      <c r="AB25" s="25"/>
+      <c r="AB25" s="18"/>
     </row>
     <row r="26" spans="2:28">
       <c r="B26" s="10"/>
@@ -2427,7 +2506,7 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
-      <c r="AB26" s="25"/>
+      <c r="AB26" s="18"/>
     </row>
     <row r="27" spans="2:28">
       <c r="B27" s="10"/>
@@ -2456,7 +2535,7 @@
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
-      <c r="AB27" s="25"/>
+      <c r="AB27" s="18"/>
     </row>
     <row r="28" spans="2:28">
       <c r="B28" s="10"/>
@@ -2485,7 +2564,7 @@
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
       <c r="AA28" s="12"/>
-      <c r="AB28" s="25"/>
+      <c r="AB28" s="18"/>
     </row>
     <row r="29" spans="2:28">
       <c r="B29" s="10"/>
@@ -2514,11 +2593,11 @@
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
       <c r="AA29" s="12"/>
-      <c r="AB29" s="25"/>
+      <c r="AB29" s="18"/>
     </row>
     <row r="30" ht="15" spans="2:28">
       <c r="B30" s="10"/>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="12" t="s">
@@ -2546,11 +2625,11 @@
       <c r="Y30" s="12"/>
       <c r="Z30" s="12"/>
       <c r="AA30" s="12"/>
-      <c r="AB30" s="25"/>
+      <c r="AB30" s="18"/>
     </row>
     <row r="31" ht="15" spans="2:28">
       <c r="B31" s="10"/>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="12" t="s">
@@ -2578,11 +2657,11 @@
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
       <c r="AA31" s="12"/>
-      <c r="AB31" s="25"/>
+      <c r="AB31" s="18"/>
     </row>
     <row r="32" ht="15" spans="2:28">
       <c r="B32" s="10"/>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="12" t="s">
@@ -2610,7 +2689,7 @@
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
       <c r="AA32" s="12"/>
-      <c r="AB32" s="25"/>
+      <c r="AB32" s="18"/>
     </row>
     <row r="33" spans="2:28">
       <c r="B33" s="10"/>
@@ -2639,11 +2718,11 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="12"/>
-      <c r="AB33" s="25"/>
+      <c r="AB33" s="18"/>
     </row>
     <row r="34" ht="20.1" customHeight="1" spans="2:28">
       <c r="B34" s="8"/>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -2672,7 +2751,7 @@
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
       <c r="AA34" s="9"/>
-      <c r="AB34" s="24"/>
+      <c r="AB34" s="17"/>
     </row>
     <row r="35" spans="2:28">
       <c r="B35" s="10"/>
@@ -2701,7 +2780,7 @@
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
       <c r="AA35" s="12"/>
-      <c r="AB35" s="25"/>
+      <c r="AB35" s="18"/>
     </row>
     <row r="36" ht="15" spans="2:28">
       <c r="B36" s="10"/>
@@ -2734,7 +2813,7 @@
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
       <c r="AA36" s="12"/>
-      <c r="AB36" s="25"/>
+      <c r="AB36" s="18"/>
     </row>
     <row r="37" ht="15" spans="2:28">
       <c r="B37" s="10"/>
@@ -2767,7 +2846,7 @@
       <c r="Y37" s="12"/>
       <c r="Z37" s="12"/>
       <c r="AA37" s="12"/>
-      <c r="AB37" s="25"/>
+      <c r="AB37" s="18"/>
     </row>
     <row r="38" ht="15" spans="2:28">
       <c r="B38" s="10"/>
@@ -2800,7 +2879,7 @@
       <c r="Y38" s="12"/>
       <c r="Z38" s="12"/>
       <c r="AA38" s="12"/>
-      <c r="AB38" s="25"/>
+      <c r="AB38" s="18"/>
     </row>
     <row r="39" ht="15" spans="2:28">
       <c r="B39" s="10"/>
@@ -2833,7 +2912,7 @@
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
       <c r="AA39" s="12"/>
-      <c r="AB39" s="25"/>
+      <c r="AB39" s="18"/>
     </row>
     <row r="40" spans="2:28">
       <c r="B40" s="10"/>
@@ -2862,11 +2941,11 @@
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
       <c r="AA40" s="12"/>
-      <c r="AB40" s="25"/>
+      <c r="AB40" s="18"/>
     </row>
     <row r="41" ht="20.1" customHeight="1" spans="2:28">
       <c r="B41" s="8"/>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="30" t="s">
         <v>20</v>
       </c>
       <c r="D41" s="9" t="s">
@@ -2895,319 +2974,319 @@
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
       <c r="AA41" s="9"/>
-      <c r="AB41" s="24"/>
+      <c r="AB41" s="17"/>
     </row>
     <row r="42" spans="2:28">
-      <c r="B42" s="29"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="31"/>
-      <c r="Q42" s="31"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="31"/>
-      <c r="U42" s="31"/>
-      <c r="V42" s="31"/>
-      <c r="W42" s="31"/>
-      <c r="X42" s="31"/>
-      <c r="Y42" s="31"/>
-      <c r="Z42" s="31"/>
-      <c r="AA42" s="31"/>
-      <c r="AB42" s="32"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12"/>
+      <c r="V42" s="12"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="12"/>
+      <c r="Y42" s="12"/>
+      <c r="Z42" s="12"/>
+      <c r="AA42" s="12"/>
+      <c r="AB42" s="18"/>
     </row>
     <row r="43" ht="15" spans="2:28">
-      <c r="B43" s="29"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="31"/>
-      <c r="U43" s="31"/>
-      <c r="V43" s="31"/>
-      <c r="W43" s="31"/>
-      <c r="X43" s="31"/>
-      <c r="Y43" s="31"/>
-      <c r="Z43" s="31"/>
-      <c r="AA43" s="31"/>
-      <c r="AB43" s="32"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
+      <c r="S43" s="12"/>
+      <c r="T43" s="12"/>
+      <c r="U43" s="12"/>
+      <c r="V43" s="12"/>
+      <c r="W43" s="12"/>
+      <c r="X43" s="12"/>
+      <c r="Y43" s="12"/>
+      <c r="Z43" s="12"/>
+      <c r="AA43" s="12"/>
+      <c r="AB43" s="18"/>
     </row>
     <row r="44" ht="15" spans="2:28">
-      <c r="B44" s="29"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
-      <c r="P44" s="31"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
-      <c r="S44" s="31"/>
-      <c r="T44" s="31"/>
-      <c r="U44" s="31"/>
-      <c r="V44" s="31"/>
-      <c r="W44" s="31"/>
-      <c r="X44" s="31"/>
-      <c r="Y44" s="31"/>
-      <c r="Z44" s="31"/>
-      <c r="AA44" s="31"/>
-      <c r="AB44" s="32"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="12"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="18"/>
     </row>
     <row r="45" ht="15" spans="2:28">
-      <c r="B45" s="29"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
-      <c r="O45" s="31"/>
-      <c r="P45" s="31"/>
-      <c r="Q45" s="31"/>
-      <c r="R45" s="31"/>
-      <c r="S45" s="31"/>
-      <c r="T45" s="31"/>
-      <c r="U45" s="31"/>
-      <c r="V45" s="31"/>
-      <c r="W45" s="31"/>
-      <c r="X45" s="31"/>
-      <c r="Y45" s="31"/>
-      <c r="Z45" s="31"/>
-      <c r="AA45" s="31"/>
-      <c r="AB45" s="32"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="18"/>
     </row>
     <row r="46" spans="2:28">
-      <c r="B46" s="29"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="31" t="s">
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
-      <c r="P46" s="31"/>
-      <c r="Q46" s="31"/>
-      <c r="R46" s="31"/>
-      <c r="S46" s="31"/>
-      <c r="T46" s="31"/>
-      <c r="U46" s="31"/>
-      <c r="V46" s="31"/>
-      <c r="W46" s="31"/>
-      <c r="X46" s="31"/>
-      <c r="Y46" s="31"/>
-      <c r="Z46" s="31"/>
-      <c r="AA46" s="31"/>
-      <c r="AB46" s="32"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="18"/>
     </row>
     <row r="47" spans="2:28">
-      <c r="B47" s="29"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31" t="s">
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="31"/>
-      <c r="S47" s="31"/>
-      <c r="T47" s="31"/>
-      <c r="U47" s="31"/>
-      <c r="V47" s="31"/>
-      <c r="W47" s="31"/>
-      <c r="X47" s="31"/>
-      <c r="Y47" s="31"/>
-      <c r="Z47" s="31"/>
-      <c r="AA47" s="31"/>
-      <c r="AB47" s="32"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
+      <c r="U47" s="12"/>
+      <c r="V47" s="12"/>
+      <c r="W47" s="12"/>
+      <c r="X47" s="12"/>
+      <c r="Y47" s="12"/>
+      <c r="Z47" s="12"/>
+      <c r="AA47" s="12"/>
+      <c r="AB47" s="18"/>
     </row>
     <row r="48" spans="2:28">
-      <c r="B48" s="29"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="31" t="s">
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
-      <c r="K48" s="31"/>
-      <c r="L48" s="31"/>
-      <c r="M48" s="31"/>
-      <c r="N48" s="31"/>
-      <c r="O48" s="31"/>
-      <c r="P48" s="31"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="31"/>
-      <c r="S48" s="31"/>
-      <c r="T48" s="31"/>
-      <c r="U48" s="31"/>
-      <c r="V48" s="31"/>
-      <c r="W48" s="31"/>
-      <c r="X48" s="31"/>
-      <c r="Y48" s="31"/>
-      <c r="Z48" s="31"/>
-      <c r="AA48" s="31"/>
-      <c r="AB48" s="32"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+      <c r="S48" s="12"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="12"/>
+      <c r="V48" s="12"/>
+      <c r="W48" s="12"/>
+      <c r="X48" s="12"/>
+      <c r="Y48" s="12"/>
+      <c r="Z48" s="12"/>
+      <c r="AA48" s="12"/>
+      <c r="AB48" s="18"/>
     </row>
     <row r="49" ht="15" spans="2:28">
-      <c r="B49" s="29"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="31"/>
-      <c r="K49" s="31"/>
-      <c r="L49" s="31"/>
-      <c r="M49" s="31"/>
-      <c r="N49" s="31"/>
-      <c r="O49" s="31"/>
-      <c r="P49" s="31"/>
-      <c r="Q49" s="31"/>
-      <c r="R49" s="31"/>
-      <c r="S49" s="31"/>
-      <c r="T49" s="31"/>
-      <c r="U49" s="31"/>
-      <c r="V49" s="31"/>
-      <c r="W49" s="31"/>
-      <c r="X49" s="31"/>
-      <c r="Y49" s="31"/>
-      <c r="Z49" s="31"/>
-      <c r="AA49" s="31"/>
-      <c r="AB49" s="32"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="12"/>
+      <c r="V49" s="12"/>
+      <c r="W49" s="12"/>
+      <c r="X49" s="12"/>
+      <c r="Y49" s="12"/>
+      <c r="Z49" s="12"/>
+      <c r="AA49" s="12"/>
+      <c r="AB49" s="18"/>
     </row>
     <row r="50" spans="2:28">
-      <c r="B50" s="29"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
-      <c r="P50" s="31"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="31"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="31"/>
-      <c r="U50" s="31"/>
-      <c r="V50" s="31"/>
-      <c r="W50" s="31"/>
-      <c r="X50" s="31"/>
-      <c r="Y50" s="31"/>
-      <c r="Z50" s="31"/>
-      <c r="AA50" s="31"/>
-      <c r="AB50" s="32"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="12"/>
+      <c r="V50" s="12"/>
+      <c r="W50" s="12"/>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="12"/>
+      <c r="Z50" s="12"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="18"/>
     </row>
     <row r="51" ht="14.55" customHeight="1" spans="2:28">
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
-      <c r="S51" s="21"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
-      <c r="V51" s="21"/>
-      <c r="W51" s="21"/>
-      <c r="X51" s="21"/>
-      <c r="Y51" s="21"/>
-      <c r="Z51" s="21"/>
-      <c r="AA51" s="21"/>
-      <c r="AB51" s="26"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="23"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="23"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="23"/>
+      <c r="W51" s="23"/>
+      <c r="X51" s="23"/>
+      <c r="Y51" s="23"/>
+      <c r="Z51" s="23"/>
+      <c r="AA51" s="23"/>
+      <c r="AB51" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3225,7 +3304,7 @@
   <sheetPr/>
   <dimension ref="B1:AB47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3268,7 +3347,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
-      <c r="AB1" s="22"/>
+      <c r="AB1" s="15"/>
     </row>
     <row r="2" spans="2:28">
       <c r="B2" s="6"/>
@@ -3297,7 +3376,7 @@
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
-      <c r="AB2" s="23"/>
+      <c r="AB2" s="16"/>
     </row>
     <row r="3" spans="2:28">
       <c r="B3" s="6"/>
@@ -3326,11 +3405,11 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AB3" s="23"/>
+      <c r="AB3" s="16"/>
     </row>
     <row r="4" ht="20.1" customHeight="1" spans="2:28">
       <c r="B4" s="8"/>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -3359,7 +3438,7 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
-      <c r="AB4" s="24"/>
+      <c r="AB4" s="17"/>
     </row>
     <row r="5" spans="2:28">
       <c r="B5" s="10"/>
@@ -3388,11 +3467,11 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
-      <c r="AB5" s="25"/>
+      <c r="AB5" s="18"/>
     </row>
     <row r="6" spans="2:28">
       <c r="B6" s="10"/>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="12"/>
@@ -3419,7 +3498,7 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="12"/>
-      <c r="AB6" s="25"/>
+      <c r="AB6" s="18"/>
     </row>
     <row r="7" spans="2:28">
       <c r="B7" s="10"/>
@@ -3448,18 +3527,18 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
-      <c r="AB7" s="25"/>
+      <c r="AB7" s="18"/>
     </row>
     <row r="8" ht="14.4" spans="2:28">
       <c r="B8" s="10"/>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -3479,7 +3558,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
-      <c r="AB8" s="25"/>
+      <c r="AB8" s="18"/>
     </row>
     <row r="9" spans="2:28">
       <c r="B9" s="10"/>
@@ -3508,7 +3587,7 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
       <c r="AA9" s="12"/>
-      <c r="AB9" s="25"/>
+      <c r="AB9" s="18"/>
     </row>
     <row r="10" spans="2:28">
       <c r="B10" s="10"/>
@@ -3537,7 +3616,7 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="12"/>
-      <c r="AB10" s="25"/>
+      <c r="AB10" s="18"/>
     </row>
     <row r="11" spans="2:28">
       <c r="B11" s="10"/>
@@ -3566,7 +3645,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
-      <c r="AB11" s="25"/>
+      <c r="AB11" s="18"/>
     </row>
     <row r="12" spans="2:28">
       <c r="B12" s="10"/>
@@ -3595,7 +3674,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
-      <c r="AB12" s="25"/>
+      <c r="AB12" s="18"/>
     </row>
     <row r="13" spans="2:28">
       <c r="B13" s="10"/>
@@ -3624,7 +3703,7 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
-      <c r="AB13" s="25"/>
+      <c r="AB13" s="18"/>
     </row>
     <row r="14" spans="2:28">
       <c r="B14" s="10"/>
@@ -3653,7 +3732,7 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
       <c r="AA14" s="12"/>
-      <c r="AB14" s="25"/>
+      <c r="AB14" s="18"/>
     </row>
     <row r="15" spans="2:28">
       <c r="B15" s="10"/>
@@ -3682,7 +3761,7 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
-      <c r="AB15" s="25"/>
+      <c r="AB15" s="18"/>
     </row>
     <row r="16" spans="2:28">
       <c r="B16" s="10"/>
@@ -3711,7 +3790,7 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
-      <c r="AB16" s="25"/>
+      <c r="AB16" s="18"/>
     </row>
     <row r="17" spans="2:28">
       <c r="B17" s="10"/>
@@ -3740,7 +3819,7 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
-      <c r="AB17" s="25"/>
+      <c r="AB17" s="18"/>
     </row>
     <row r="18" spans="2:28">
       <c r="B18" s="10"/>
@@ -3769,7 +3848,7 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
-      <c r="AB18" s="25"/>
+      <c r="AB18" s="18"/>
     </row>
     <row r="19" spans="2:28">
       <c r="B19" s="10"/>
@@ -3798,7 +3877,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
-      <c r="AB19" s="25"/>
+      <c r="AB19" s="18"/>
     </row>
     <row r="20" spans="2:28">
       <c r="B20" s="10"/>
@@ -3827,7 +3906,7 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
-      <c r="AB20" s="25"/>
+      <c r="AB20" s="18"/>
     </row>
     <row r="21" spans="2:28">
       <c r="B21" s="10"/>
@@ -3856,7 +3935,7 @@
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
-      <c r="AB21" s="25"/>
+      <c r="AB21" s="18"/>
     </row>
     <row r="22" spans="2:28">
       <c r="B22" s="10"/>
@@ -3885,7 +3964,7 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
-      <c r="AB22" s="25"/>
+      <c r="AB22" s="18"/>
     </row>
     <row r="23" spans="2:28">
       <c r="B23" s="10"/>
@@ -3914,7 +3993,7 @@
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
       <c r="AA23" s="12"/>
-      <c r="AB23" s="25"/>
+      <c r="AB23" s="18"/>
     </row>
     <row r="24" spans="2:28">
       <c r="B24" s="10"/>
@@ -3943,7 +4022,7 @@
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
       <c r="AA24" s="12"/>
-      <c r="AB24" s="25"/>
+      <c r="AB24" s="18"/>
     </row>
     <row r="25" spans="2:28">
       <c r="B25" s="10"/>
@@ -3972,7 +4051,7 @@
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
       <c r="AA25" s="12"/>
-      <c r="AB25" s="25"/>
+      <c r="AB25" s="18"/>
     </row>
     <row r="26" spans="2:28">
       <c r="B26" s="10"/>
@@ -4001,7 +4080,7 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
-      <c r="AB26" s="25"/>
+      <c r="AB26" s="18"/>
     </row>
     <row r="27" spans="2:28">
       <c r="B27" s="10"/>
@@ -4030,7 +4109,7 @@
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
-      <c r="AB27" s="25"/>
+      <c r="AB27" s="18"/>
     </row>
     <row r="28" spans="2:28">
       <c r="B28" s="10"/>
@@ -4059,7 +4138,7 @@
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
       <c r="AA28" s="12"/>
-      <c r="AB28" s="25"/>
+      <c r="AB28" s="18"/>
     </row>
     <row r="29" spans="2:28">
       <c r="B29" s="10"/>
@@ -4088,7 +4167,7 @@
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
       <c r="AA29" s="12"/>
-      <c r="AB29" s="25"/>
+      <c r="AB29" s="18"/>
     </row>
     <row r="30" spans="2:28">
       <c r="B30" s="10"/>
@@ -4117,7 +4196,7 @@
       <c r="Y30" s="12"/>
       <c r="Z30" s="12"/>
       <c r="AA30" s="12"/>
-      <c r="AB30" s="25"/>
+      <c r="AB30" s="18"/>
     </row>
     <row r="31" spans="2:28">
       <c r="B31" s="10"/>
@@ -4146,7 +4225,7 @@
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
       <c r="AA31" s="12"/>
-      <c r="AB31" s="25"/>
+      <c r="AB31" s="18"/>
     </row>
     <row r="32" spans="2:28">
       <c r="B32" s="10"/>
@@ -4175,7 +4254,7 @@
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
       <c r="AA32" s="12"/>
-      <c r="AB32" s="25"/>
+      <c r="AB32" s="18"/>
     </row>
     <row r="33" spans="2:28">
       <c r="B33" s="10"/>
@@ -4204,11 +4283,11 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="12"/>
-      <c r="AB33" s="25"/>
+      <c r="AB33" s="18"/>
     </row>
     <row r="34" spans="2:28">
       <c r="B34" s="10"/>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D34" s="12"/>
@@ -4235,7 +4314,7 @@
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
       <c r="AA34" s="12"/>
-      <c r="AB34" s="25"/>
+      <c r="AB34" s="18"/>
     </row>
     <row r="35" spans="2:28">
       <c r="B35" s="10"/>
@@ -4263,7 +4342,7 @@
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
       <c r="AA35" s="12"/>
-      <c r="AB35" s="25"/>
+      <c r="AB35" s="18"/>
     </row>
     <row r="36" ht="14.4" spans="2:28">
       <c r="B36" s="10"/>
@@ -4294,7 +4373,7 @@
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
       <c r="AA36" s="12"/>
-      <c r="AB36" s="25"/>
+      <c r="AB36" s="18"/>
     </row>
     <row r="37" ht="14.4" spans="2:28">
       <c r="B37" s="10"/>
@@ -4323,11 +4402,11 @@
       <c r="Y37" s="12"/>
       <c r="Z37" s="12"/>
       <c r="AA37" s="12"/>
-      <c r="AB37" s="25"/>
+      <c r="AB37" s="18"/>
     </row>
     <row r="38" ht="20.1" customHeight="1" spans="2:28">
       <c r="B38" s="8"/>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -4356,7 +4435,7 @@
       <c r="Y38" s="9"/>
       <c r="Z38" s="9"/>
       <c r="AA38" s="9"/>
-      <c r="AB38" s="24"/>
+      <c r="AB38" s="17"/>
     </row>
     <row r="39" ht="14.4" spans="2:28">
       <c r="B39" s="10"/>
@@ -4385,11 +4464,11 @@
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
       <c r="AA39" s="12"/>
-      <c r="AB39" s="25"/>
+      <c r="AB39" s="18"/>
     </row>
     <row r="40" ht="14.4" spans="2:28">
       <c r="B40" s="10"/>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="19" t="s">
         <v>35</v>
       </c>
       <c r="D40" s="12"/>
@@ -4416,7 +4495,7 @@
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
       <c r="AA40" s="12"/>
-      <c r="AB40" s="25"/>
+      <c r="AB40" s="18"/>
     </row>
     <row r="41" ht="14.4" spans="2:28">
       <c r="B41" s="10"/>
@@ -4445,7 +4524,7 @@
       <c r="Y41" s="12"/>
       <c r="Z41" s="12"/>
       <c r="AA41" s="12"/>
-      <c r="AB41" s="25"/>
+      <c r="AB41" s="18"/>
     </row>
     <row r="42" spans="2:28">
       <c r="B42" s="10"/>
@@ -4474,11 +4553,11 @@
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
       <c r="AA42" s="12"/>
-      <c r="AB42" s="25"/>
+      <c r="AB42" s="18"/>
     </row>
     <row r="43" ht="20.1" customHeight="1" spans="2:28">
       <c r="B43" s="8"/>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="9" t="s">
@@ -4507,7 +4586,7 @@
       <c r="Y43" s="9"/>
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
-      <c r="AB43" s="24"/>
+      <c r="AB43" s="17"/>
     </row>
     <row r="44" spans="2:28">
       <c r="B44" s="10"/>
@@ -4536,11 +4615,11 @@
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
       <c r="AA44" s="12"/>
-      <c r="AB44" s="25"/>
+      <c r="AB44" s="18"/>
     </row>
     <row r="45" ht="14.4" spans="2:28">
       <c r="B45" s="10"/>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="20" t="s">
         <v>37</v>
       </c>
       <c r="D45" s="12"/>
@@ -4567,7 +4646,7 @@
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
       <c r="AA45" s="12"/>
-      <c r="AB45" s="25"/>
+      <c r="AB45" s="18"/>
     </row>
     <row r="46" spans="2:28">
       <c r="B46" s="10"/>
@@ -4596,36 +4675,36 @@
       <c r="Y46" s="12"/>
       <c r="Z46" s="12"/>
       <c r="AA46" s="12"/>
-      <c r="AB46" s="25"/>
+      <c r="AB46" s="18"/>
     </row>
     <row r="47" ht="14.55" spans="2:28">
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
-      <c r="Q47" s="21"/>
-      <c r="R47" s="21"/>
-      <c r="S47" s="21"/>
-      <c r="T47" s="21"/>
-      <c r="U47" s="21"/>
-      <c r="V47" s="21"/>
-      <c r="W47" s="21"/>
-      <c r="X47" s="21"/>
-      <c r="Y47" s="21"/>
-      <c r="Z47" s="21"/>
-      <c r="AA47" s="21"/>
-      <c r="AB47" s="26"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="23"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="23"/>
+      <c r="S47" s="23"/>
+      <c r="T47" s="23"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="23"/>
+      <c r="W47" s="23"/>
+      <c r="X47" s="23"/>
+      <c r="Y47" s="23"/>
+      <c r="Z47" s="23"/>
+      <c r="AA47" s="23"/>
+      <c r="AB47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4641,4 +4720,2148 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:AB72"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.62962962962963" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="2.62962962962963" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.62962962962963" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.62962962962963" style="2"/>
+    <col min="4" max="28" width="4.62962962962963" style="1"/>
+    <col min="29" max="29" width="2.62962962962963" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="4.62962962962963" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:28">
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="15"/>
+    </row>
+    <row r="2" spans="2:28">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="16"/>
+    </row>
+    <row r="3" spans="2:28">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="16"/>
+    </row>
+    <row r="4" ht="20.1" customHeight="1" spans="2:28">
+      <c r="B4" s="8"/>
+      <c r="C4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="17"/>
+    </row>
+    <row r="5" spans="2:28">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="18"/>
+    </row>
+    <row r="6" spans="2:28">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="18"/>
+    </row>
+    <row r="7" spans="2:28">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="18"/>
+    </row>
+    <row r="8" spans="2:28">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="18"/>
+    </row>
+    <row r="9" spans="2:28">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="18"/>
+    </row>
+    <row r="10" spans="2:28">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="18"/>
+    </row>
+    <row r="11" spans="2:28">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="18"/>
+    </row>
+    <row r="12" spans="2:28">
+      <c r="B12" s="10"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="18"/>
+    </row>
+    <row r="13" spans="2:28">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="18"/>
+    </row>
+    <row r="14" spans="2:28">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="18"/>
+    </row>
+    <row r="15" spans="2:28">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="18"/>
+    </row>
+    <row r="16" spans="2:28">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="18"/>
+    </row>
+    <row r="17" spans="2:28">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="18"/>
+    </row>
+    <row r="18" spans="2:28">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="18"/>
+    </row>
+    <row r="19" spans="2:28">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="18"/>
+    </row>
+    <row r="20" spans="2:28">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="18"/>
+    </row>
+    <row r="21" spans="2:28">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="18"/>
+    </row>
+    <row r="22" spans="2:28">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="18"/>
+    </row>
+    <row r="23" spans="2:28">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="18"/>
+    </row>
+    <row r="24" spans="2:28">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="12"/>
+      <c r="AB24" s="18"/>
+    </row>
+    <row r="25" spans="2:28">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="18"/>
+    </row>
+    <row r="26" spans="2:28">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="18"/>
+    </row>
+    <row r="27" spans="2:28">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="18"/>
+    </row>
+    <row r="28" spans="2:28">
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="18"/>
+    </row>
+    <row r="29" spans="2:28">
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="18"/>
+    </row>
+    <row r="30" spans="2:28">
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="18"/>
+    </row>
+    <row r="31" spans="2:28">
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="12"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="18"/>
+    </row>
+    <row r="32" spans="2:28">
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="18"/>
+    </row>
+    <row r="33" spans="2:28">
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="18"/>
+    </row>
+    <row r="34" spans="2:28">
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="18"/>
+    </row>
+    <row r="35" spans="2:28">
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="18"/>
+    </row>
+    <row r="36" spans="2:28">
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="18"/>
+    </row>
+    <row r="37" spans="2:28">
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12"/>
+      <c r="V37" s="12"/>
+      <c r="W37" s="12"/>
+      <c r="X37" s="12"/>
+      <c r="Y37" s="12"/>
+      <c r="Z37" s="12"/>
+      <c r="AA37" s="12"/>
+      <c r="AB37" s="18"/>
+    </row>
+    <row r="38" spans="2:28">
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
+      <c r="V38" s="12"/>
+      <c r="W38" s="12"/>
+      <c r="X38" s="12"/>
+      <c r="Y38" s="12"/>
+      <c r="Z38" s="12"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="18"/>
+    </row>
+    <row r="39" spans="2:28">
+      <c r="B39" s="10"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12"/>
+      <c r="W39" s="12"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="12"/>
+      <c r="Z39" s="12"/>
+      <c r="AA39" s="12"/>
+      <c r="AB39" s="18"/>
+    </row>
+    <row r="40" spans="2:28">
+      <c r="B40" s="10"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
+      <c r="U40" s="12"/>
+      <c r="V40" s="12"/>
+      <c r="W40" s="12"/>
+      <c r="X40" s="12"/>
+      <c r="Y40" s="12"/>
+      <c r="Z40" s="12"/>
+      <c r="AA40" s="12"/>
+      <c r="AB40" s="18"/>
+    </row>
+    <row r="41" ht="14.4" spans="2:28">
+      <c r="B41" s="10"/>
+      <c r="C41"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="12"/>
+      <c r="Z41" s="12"/>
+      <c r="AA41" s="12"/>
+      <c r="AB41" s="18"/>
+    </row>
+    <row r="42" ht="14.4" spans="2:28">
+      <c r="B42" s="10"/>
+      <c r="C42"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12"/>
+      <c r="V42" s="12"/>
+      <c r="W42" s="12"/>
+      <c r="X42" s="12"/>
+      <c r="Y42" s="12"/>
+      <c r="Z42" s="12"/>
+      <c r="AA42" s="12"/>
+      <c r="AB42" s="18"/>
+    </row>
+    <row r="43" ht="20.1" customHeight="1" spans="2:28">
+      <c r="B43" s="8"/>
+      <c r="C43" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
+      <c r="Z43" s="9"/>
+      <c r="AA43" s="9"/>
+      <c r="AB43" s="17"/>
+    </row>
+    <row r="44" ht="14.4" spans="2:28">
+      <c r="B44" s="10"/>
+      <c r="C44"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="12"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="18"/>
+    </row>
+    <row r="45" ht="14.4" spans="2:28">
+      <c r="B45" s="10"/>
+      <c r="C45"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="18"/>
+    </row>
+    <row r="46" ht="14.4" spans="2:28">
+      <c r="B46" s="10"/>
+      <c r="C46"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="18"/>
+    </row>
+    <row r="47" ht="14.4" spans="2:28">
+      <c r="B47" s="10"/>
+      <c r="C47"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
+      <c r="U47" s="12"/>
+      <c r="V47" s="12"/>
+      <c r="W47" s="12"/>
+      <c r="X47" s="12"/>
+      <c r="Y47" s="12"/>
+      <c r="Z47" s="12"/>
+      <c r="AA47" s="12"/>
+      <c r="AB47" s="18"/>
+    </row>
+    <row r="48" ht="14.4" spans="2:28">
+      <c r="B48" s="10"/>
+      <c r="C48"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+      <c r="S48" s="12"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="12"/>
+      <c r="V48" s="12"/>
+      <c r="W48" s="12"/>
+      <c r="X48" s="12"/>
+      <c r="Y48" s="12"/>
+      <c r="Z48" s="12"/>
+      <c r="AA48" s="12"/>
+      <c r="AB48" s="18"/>
+    </row>
+    <row r="49" ht="14.4" spans="2:28">
+      <c r="B49" s="10"/>
+      <c r="C49"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="12"/>
+      <c r="V49" s="12"/>
+      <c r="W49" s="12"/>
+      <c r="X49" s="12"/>
+      <c r="Y49" s="12"/>
+      <c r="Z49" s="12"/>
+      <c r="AA49" s="12"/>
+      <c r="AB49" s="18"/>
+    </row>
+    <row r="50" ht="14.4" spans="2:28">
+      <c r="B50" s="10"/>
+      <c r="C50"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="12"/>
+      <c r="V50" s="12"/>
+      <c r="W50" s="12"/>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="12"/>
+      <c r="Z50" s="12"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="18"/>
+    </row>
+    <row r="51" ht="14.4" spans="2:28">
+      <c r="B51" s="10"/>
+      <c r="C51"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="X51" s="12"/>
+      <c r="Y51" s="12"/>
+      <c r="Z51" s="12"/>
+      <c r="AA51" s="12"/>
+      <c r="AB51" s="18"/>
+    </row>
+    <row r="52" ht="14.4" spans="2:28">
+      <c r="B52" s="10"/>
+      <c r="C52"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="12"/>
+      <c r="X52" s="12"/>
+      <c r="Y52" s="12"/>
+      <c r="Z52" s="12"/>
+      <c r="AA52" s="12"/>
+      <c r="AB52" s="18"/>
+    </row>
+    <row r="53" ht="14.4" spans="2:28">
+      <c r="B53" s="10"/>
+      <c r="C53"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="12"/>
+      <c r="T53" s="12"/>
+      <c r="U53" s="12"/>
+      <c r="V53" s="12"/>
+      <c r="W53" s="12"/>
+      <c r="X53" s="12"/>
+      <c r="Y53" s="12"/>
+      <c r="Z53" s="12"/>
+      <c r="AA53" s="12"/>
+      <c r="AB53" s="18"/>
+    </row>
+    <row r="54" ht="14.4" spans="2:28">
+      <c r="B54" s="10"/>
+      <c r="C54"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="12"/>
+      <c r="T54" s="12"/>
+      <c r="U54" s="12"/>
+      <c r="V54" s="12"/>
+      <c r="W54" s="12"/>
+      <c r="X54" s="12"/>
+      <c r="Y54" s="12"/>
+      <c r="Z54" s="12"/>
+      <c r="AA54" s="12"/>
+      <c r="AB54" s="18"/>
+    </row>
+    <row r="55" ht="14.4" spans="2:28">
+      <c r="B55" s="10"/>
+      <c r="C55"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="12"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="12"/>
+      <c r="V55" s="12"/>
+      <c r="W55" s="12"/>
+      <c r="X55" s="12"/>
+      <c r="Y55" s="12"/>
+      <c r="Z55" s="12"/>
+      <c r="AA55" s="12"/>
+      <c r="AB55" s="18"/>
+    </row>
+    <row r="56" ht="14.4" spans="2:28">
+      <c r="B56" s="10"/>
+      <c r="C56"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="12"/>
+      <c r="V56" s="12"/>
+      <c r="W56" s="12"/>
+      <c r="X56" s="12"/>
+      <c r="Y56" s="12"/>
+      <c r="Z56" s="12"/>
+      <c r="AA56" s="12"/>
+      <c r="AB56" s="18"/>
+    </row>
+    <row r="57" ht="14.4" spans="2:28">
+      <c r="B57" s="10"/>
+      <c r="C57"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="12"/>
+      <c r="U57" s="12"/>
+      <c r="V57" s="12"/>
+      <c r="W57" s="12"/>
+      <c r="X57" s="12"/>
+      <c r="Y57" s="12"/>
+      <c r="Z57" s="12"/>
+      <c r="AA57" s="12"/>
+      <c r="AB57" s="18"/>
+    </row>
+    <row r="58" ht="14.4" spans="2:28">
+      <c r="B58" s="10"/>
+      <c r="C58"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="12"/>
+      <c r="T58" s="12"/>
+      <c r="U58" s="12"/>
+      <c r="V58" s="12"/>
+      <c r="W58" s="12"/>
+      <c r="X58" s="12"/>
+      <c r="Y58" s="12"/>
+      <c r="Z58" s="12"/>
+      <c r="AA58" s="12"/>
+      <c r="AB58" s="18"/>
+    </row>
+    <row r="59" ht="14.4" spans="2:28">
+      <c r="B59" s="10"/>
+      <c r="C59"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="12"/>
+      <c r="N59" s="12"/>
+      <c r="O59" s="12"/>
+      <c r="P59" s="12"/>
+      <c r="Q59" s="12"/>
+      <c r="R59" s="12"/>
+      <c r="S59" s="12"/>
+      <c r="T59" s="12"/>
+      <c r="U59" s="12"/>
+      <c r="V59" s="12"/>
+      <c r="W59" s="12"/>
+      <c r="X59" s="12"/>
+      <c r="Y59" s="12"/>
+      <c r="Z59" s="12"/>
+      <c r="AA59" s="12"/>
+      <c r="AB59" s="18"/>
+    </row>
+    <row r="60" ht="14.4" spans="2:28">
+      <c r="B60" s="10"/>
+      <c r="C60"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
+      <c r="R60" s="12"/>
+      <c r="S60" s="12"/>
+      <c r="T60" s="12"/>
+      <c r="U60" s="12"/>
+      <c r="V60" s="12"/>
+      <c r="W60" s="12"/>
+      <c r="X60" s="12"/>
+      <c r="Y60" s="12"/>
+      <c r="Z60" s="12"/>
+      <c r="AA60" s="12"/>
+      <c r="AB60" s="18"/>
+    </row>
+    <row r="61" ht="14.4" spans="2:28">
+      <c r="B61" s="10"/>
+      <c r="C61"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12"/>
+      <c r="R61" s="12"/>
+      <c r="S61" s="12"/>
+      <c r="T61" s="12"/>
+      <c r="U61" s="12"/>
+      <c r="V61" s="12"/>
+      <c r="W61" s="12"/>
+      <c r="X61" s="12"/>
+      <c r="Y61" s="12"/>
+      <c r="Z61" s="12"/>
+      <c r="AA61" s="12"/>
+      <c r="AB61" s="18"/>
+    </row>
+    <row r="62" ht="14.4" spans="2:28">
+      <c r="B62" s="10"/>
+      <c r="C62"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="12"/>
+      <c r="T62" s="12"/>
+      <c r="U62" s="12"/>
+      <c r="V62" s="12"/>
+      <c r="W62" s="12"/>
+      <c r="X62" s="12"/>
+      <c r="Y62" s="12"/>
+      <c r="Z62" s="12"/>
+      <c r="AA62" s="12"/>
+      <c r="AB62" s="18"/>
+    </row>
+    <row r="63" ht="14.4" spans="2:28">
+      <c r="B63" s="10"/>
+      <c r="C63"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12"/>
+      <c r="R63" s="12"/>
+      <c r="S63" s="12"/>
+      <c r="T63" s="12"/>
+      <c r="U63" s="12"/>
+      <c r="V63" s="12"/>
+      <c r="W63" s="12"/>
+      <c r="X63" s="12"/>
+      <c r="Y63" s="12"/>
+      <c r="Z63" s="12"/>
+      <c r="AA63" s="12"/>
+      <c r="AB63" s="18"/>
+    </row>
+    <row r="64" ht="14.4" spans="2:28">
+      <c r="B64" s="10"/>
+      <c r="C64"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12"/>
+      <c r="T64" s="12"/>
+      <c r="U64" s="12"/>
+      <c r="V64" s="12"/>
+      <c r="W64" s="12"/>
+      <c r="X64" s="12"/>
+      <c r="Y64" s="12"/>
+      <c r="Z64" s="12"/>
+      <c r="AA64" s="12"/>
+      <c r="AB64" s="18"/>
+    </row>
+    <row r="65" ht="14.4" spans="2:28">
+      <c r="B65" s="10"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12"/>
+      <c r="R65" s="12"/>
+      <c r="S65" s="12"/>
+      <c r="T65" s="12"/>
+      <c r="U65" s="12"/>
+      <c r="V65" s="12"/>
+      <c r="W65" s="12"/>
+      <c r="X65" s="12"/>
+      <c r="Y65" s="12"/>
+      <c r="Z65" s="12"/>
+      <c r="AA65" s="12"/>
+      <c r="AB65" s="18"/>
+    </row>
+    <row r="66" ht="14.4" spans="2:28">
+      <c r="B66" s="10"/>
+      <c r="C66"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="12"/>
+      <c r="S66" s="12"/>
+      <c r="T66" s="12"/>
+      <c r="U66" s="12"/>
+      <c r="V66" s="12"/>
+      <c r="W66" s="12"/>
+      <c r="X66" s="12"/>
+      <c r="Y66" s="12"/>
+      <c r="Z66" s="12"/>
+      <c r="AA66" s="12"/>
+      <c r="AB66" s="18"/>
+    </row>
+    <row r="67" spans="2:28">
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12"/>
+      <c r="P67" s="12"/>
+      <c r="Q67" s="12"/>
+      <c r="R67" s="12"/>
+      <c r="S67" s="12"/>
+      <c r="T67" s="12"/>
+      <c r="U67" s="12"/>
+      <c r="V67" s="12"/>
+      <c r="W67" s="12"/>
+      <c r="X67" s="12"/>
+      <c r="Y67" s="12"/>
+      <c r="Z67" s="12"/>
+      <c r="AA67" s="12"/>
+      <c r="AB67" s="18"/>
+    </row>
+    <row r="68" ht="20.1" customHeight="1" spans="2:28">
+      <c r="B68" s="8"/>
+      <c r="C68" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="9"/>
+      <c r="S68" s="9"/>
+      <c r="T68" s="9"/>
+      <c r="U68" s="9"/>
+      <c r="V68" s="9"/>
+      <c r="W68" s="9"/>
+      <c r="X68" s="9"/>
+      <c r="Y68" s="9"/>
+      <c r="Z68" s="9"/>
+      <c r="AA68" s="9"/>
+      <c r="AB68" s="17"/>
+    </row>
+    <row r="69" spans="2:28">
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+      <c r="R69" s="12"/>
+      <c r="S69" s="12"/>
+      <c r="T69" s="12"/>
+      <c r="U69" s="12"/>
+      <c r="V69" s="12"/>
+      <c r="W69" s="12"/>
+      <c r="X69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="12"/>
+      <c r="AA69" s="12"/>
+      <c r="AB69" s="18"/>
+    </row>
+    <row r="70" ht="14.4" spans="2:28">
+      <c r="B70" s="10"/>
+      <c r="C70" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+      <c r="R70" s="12"/>
+      <c r="S70" s="12"/>
+      <c r="T70" s="12"/>
+      <c r="U70" s="12"/>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="X70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="Z70" s="12"/>
+      <c r="AA70" s="12"/>
+      <c r="AB70" s="18"/>
+    </row>
+    <row r="71" spans="2:28">
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+      <c r="R71" s="12"/>
+      <c r="S71" s="12"/>
+      <c r="T71" s="12"/>
+      <c r="U71" s="12"/>
+      <c r="V71" s="12"/>
+      <c r="W71" s="12"/>
+      <c r="X71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="Z71" s="12"/>
+      <c r="AA71" s="12"/>
+      <c r="AB71" s="18"/>
+    </row>
+    <row r="72" ht="14.55" spans="2:28">
+      <c r="B72" s="21"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="23"/>
+      <c r="K72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="23"/>
+      <c r="O72" s="23"/>
+      <c r="P72" s="23"/>
+      <c r="Q72" s="23"/>
+      <c r="R72" s="23"/>
+      <c r="S72" s="23"/>
+      <c r="T72" s="23"/>
+      <c r="U72" s="23"/>
+      <c r="V72" s="23"/>
+      <c r="W72" s="23"/>
+      <c r="X72" s="23"/>
+      <c r="Y72" s="23"/>
+      <c r="Z72" s="23"/>
+      <c r="AA72" s="23"/>
+      <c r="AB72" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:AB3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C70" r:id="rId2" display="https://www.docker.com/"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" scale="66" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>